<commit_message>
show grade, add competency, format name of active users, show requester name instant of mail id~
</commit_message>
<xml_diff>
--- a/ytms-cli/src/assets/excel/SampleBulkUploadFile.xlsx
+++ b/ytms-cli/src/assets/excel/SampleBulkUploadFile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20407"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aakash.sanap\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YTMS\ytms-cli\ytms-cli\src\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B912A121-C6A0-4F76-885A-60404B8219D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD2A3286-B26A-4FE0-AB0C-FFC5A0551A2B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Emp ID</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>INDORE</t>
+  </si>
+  <si>
+    <t>Competency</t>
+  </si>
+  <si>
+    <t>Java</t>
   </si>
 </sst>
 </file>
@@ -410,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1048419"/>
+  <dimension ref="A1:I1048419"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -421,9 +427,10 @@
     <col min="2" max="2" width="12.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -448,8 +455,11 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1014364</v>
       </c>
@@ -473,6 +483,9 @@
       </c>
       <c r="H2" t="s">
         <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="1048409" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>